<commit_message>
Adding Updated SLS Implicit Unit Test "test_11.py"
</commit_message>
<xml_diff>
--- a/UnitTests/TuningCorrector/test_11 Manual SLS Implicit/9/Test_11_SLS_Implicit.xlsx
+++ b/UnitTests/TuningCorrector/test_11 Manual SLS Implicit/9/Test_11_SLS_Implicit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4bda48a8e8bf62b/2021LaneLeeCCIFall2021/Data Analysis/220310_Implicit_SLS_Unit_Test_11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="537" documentId="13_ncr:40009_{2AE2FE10-F754-4E12-AD7D-77D7A5496061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB416485-6BBD-4C28-A485-27609DBF4AFB}"/>
+  <xr:revisionPtr revIDLastSave="672" documentId="13_ncr:40009_{2AE2FE10-F754-4E12-AD7D-77D7A5496061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{562F133D-9E4B-465B-BD10-3ADEB08D383B}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="20130" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="45" windowWidth="32130" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_10_SLS - Copy" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="43">
   <si>
     <t>Molecule</t>
   </si>
@@ -141,9 +141,6 @@
     <t>Ethylene (Ethene)</t>
   </si>
   <si>
-    <t>Reciprocal Correction Factor</t>
-  </si>
-  <si>
     <t>Correction factors are Highlighted:</t>
   </si>
   <si>
@@ -152,12 +149,24 @@
   <si>
     <t>Unit Test 10 Manual SLS:</t>
   </si>
+  <si>
+    <t>SLS Implicit Concetration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implicit SLS Concentration to be added: </t>
+  </si>
+  <si>
+    <t>Final Calculated Molecule Concetration:</t>
+  </si>
+  <si>
+    <t>Performing SLS Implicit:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -300,8 +309,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -502,6 +519,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -760,7 +789,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="8" applyBorder="1"/>
@@ -777,6 +806,10 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1132,15 +1165,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:V89"/>
+  <dimension ref="A2:V152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -1151,7 +1184,7 @@
   <sheetData>
     <row r="2" spans="1:22" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -1214,9 +1247,7 @@
       <c r="U7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="V7" s="13" t="s">
-        <v>36</v>
-      </c>
+      <c r="V7" s="13"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1278,10 +1309,6 @@
       </c>
       <c r="U8" s="7">
         <v>12.380758175200878</v>
-      </c>
-      <c r="V8">
-        <f>U8^-1</f>
-        <v>8.0770497723074625E-2</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1315,10 +1342,6 @@
       <c r="U9" s="8">
         <v>12.087936672079417</v>
       </c>
-      <c r="V9">
-        <f t="shared" ref="V9:V16" si="0">U9^-1</f>
-        <v>8.27271044784499E-2</v>
-      </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
@@ -1351,10 +1374,6 @@
       <c r="U10" s="8">
         <v>4.8891055066059943</v>
       </c>
-      <c r="V10">
-        <f t="shared" si="0"/>
-        <v>0.2045363919123516</v>
-      </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1387,10 +1406,6 @@
       <c r="U11" s="8">
         <v>1.187026897776684</v>
       </c>
-      <c r="V11">
-        <f t="shared" si="0"/>
-        <v>0.84244089318701398</v>
-      </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -1422,10 +1437,6 @@
       <c r="U12" s="8">
         <v>1.4227214338619145</v>
       </c>
-      <c r="V12">
-        <f t="shared" si="0"/>
-        <v>0.70287828396985919</v>
-      </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -1458,10 +1469,6 @@
       <c r="U13" s="8">
         <v>2.3997499909604523</v>
       </c>
-      <c r="V13">
-        <f t="shared" si="0"/>
-        <v>0.41671007553573108</v>
-      </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -1469,59 +1476,59 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1">
-        <f t="shared" ref="D14:Q14" si="1">D8-D13</f>
+        <f t="shared" ref="D14:Q14" si="0">D8-D13</f>
         <v>0</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.18166199999999999</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.166435</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.13122700000000001</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.8631890000000002</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.25121500000000002</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.1466E-2</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.5978000000000003E-2</v>
       </c>
       <c r="L14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.8861000000000002E-2</v>
       </c>
       <c r="M14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.173705</v>
       </c>
       <c r="N14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.4122E-2</v>
       </c>
       <c r="O14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4425E-2</v>
       </c>
       <c r="P14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-2.0010000000000002E-3</v>
       </c>
       <c r="Q14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9.9500000000000001E-4</v>
       </c>
       <c r="S14" s="5" t="s">
@@ -1532,10 +1539,6 @@
       </c>
       <c r="U14" s="8">
         <v>3.8894768008651894</v>
-      </c>
-      <c r="V14">
-        <f t="shared" si="0"/>
-        <v>0.25710398883920749</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -1548,10 +1551,6 @@
       <c r="U15" s="8">
         <v>1.0678133917468022</v>
       </c>
-      <c r="V15">
-        <f t="shared" si="0"/>
-        <v>0.93649321850527789</v>
-      </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="S16" s="9" t="s">
@@ -1563,70 +1562,66 @@
       <c r="U16" s="11">
         <v>0.55856235858755843</v>
       </c>
-      <c r="V16">
-        <f t="shared" si="0"/>
-        <v>1.7903104006662907</v>
-      </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="str">
-        <f t="shared" ref="C17:Q17" si="2">C7</f>
+        <f t="shared" ref="C17:Q17" si="1">C7</f>
         <v>Time</v>
       </c>
       <c r="D17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>m2</v>
       </c>
       <c r="E17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>m18</v>
       </c>
       <c r="F17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>m26</v>
       </c>
       <c r="G17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>m27</v>
       </c>
       <c r="H17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>m28</v>
       </c>
       <c r="I17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>m29</v>
       </c>
       <c r="J17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>m31</v>
       </c>
       <c r="K17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>m39</v>
       </c>
       <c r="L17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>m41</v>
       </c>
       <c r="M17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>m44</v>
       </c>
       <c r="N17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>m45</v>
       </c>
       <c r="O17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>m56</v>
       </c>
       <c r="P17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>m57</v>
       </c>
       <c r="Q17" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>m70</v>
       </c>
     </row>
@@ -1635,7 +1630,7 @@
         <v>24</v>
       </c>
       <c r="B18" t="str">
-        <f t="shared" ref="B18:B24" si="3">B8</f>
+        <f t="shared" ref="B18:B24" si="2">B8</f>
         <v>Remaining Signals</v>
       </c>
       <c r="C18" s="1">
@@ -1646,65 +1641,65 @@
         <v>0</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" ref="E18:Q18" si="4">E14</f>
+        <f t="shared" ref="E18:Q18" si="3">E14</f>
         <v>0.18166199999999999</v>
       </c>
       <c r="F18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.166435</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.13122700000000001</v>
       </c>
       <c r="H18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3.8631890000000002</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0.25121500000000002</v>
       </c>
       <c r="J18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>6.1466E-2</v>
       </c>
       <c r="K18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3.5978000000000003E-2</v>
       </c>
       <c r="L18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>4.8861000000000002E-2</v>
       </c>
       <c r="M18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.173705</v>
       </c>
       <c r="N18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>3.4122E-2</v>
       </c>
       <c r="O18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>1.4425E-2</v>
       </c>
       <c r="P18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-2.0010000000000002E-3</v>
       </c>
       <c r="Q18" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>9.9500000000000001E-4</v>
       </c>
       <c r="S18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="U18" s="3"/>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Correction factors</v>
       </c>
       <c r="C19" s="1"/>
@@ -1728,7 +1723,7 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Concentrations</v>
       </c>
       <c r="C20" s="1"/>
@@ -1750,13 +1745,13 @@
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
       <c r="S20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="U20" s="14"/>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>calculated main signal</v>
       </c>
       <c r="C21" s="1"/>
@@ -1780,7 +1775,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Standardized pattern</v>
       </c>
       <c r="C22" s="1"/>
@@ -1803,7 +1798,7 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>Signal to subtract</v>
       </c>
       <c r="C23" s="1"/>
@@ -1827,12 +1822,12 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>After subtraction</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1">
-        <f t="shared" ref="D24:Q24" si="5">D18-D23</f>
+        <f t="shared" ref="D24:Q24" si="4">D18-D23</f>
         <v>0</v>
       </c>
       <c r="E24" s="1">
@@ -1840,113 +1835,113 @@
         <v>0</v>
       </c>
       <c r="F24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.166435</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.13122700000000001</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.8631890000000002</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0.25121500000000002</v>
       </c>
       <c r="J24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.1466E-2</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.5978000000000003E-2</v>
       </c>
       <c r="L24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.8861000000000002E-2</v>
       </c>
       <c r="M24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.173705</v>
       </c>
       <c r="N24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.4122E-2</v>
       </c>
       <c r="O24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.4425E-2</v>
       </c>
       <c r="P24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-2.0010000000000002E-3</v>
       </c>
       <c r="Q24" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>9.9500000000000001E-4</v>
       </c>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="str">
-        <f t="shared" ref="C27:Q27" si="6">C17</f>
+        <f t="shared" ref="C27:Q27" si="5">C17</f>
         <v>Time</v>
       </c>
       <c r="D27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>m2</v>
       </c>
       <c r="E27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>m18</v>
       </c>
       <c r="F27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>m26</v>
       </c>
       <c r="G27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>m27</v>
       </c>
       <c r="H27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>m28</v>
       </c>
       <c r="I27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>m29</v>
       </c>
       <c r="J27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>m31</v>
       </c>
       <c r="K27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>m39</v>
       </c>
       <c r="L27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>m41</v>
       </c>
       <c r="M27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>m44</v>
       </c>
       <c r="N27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>m45</v>
       </c>
       <c r="O27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>m56</v>
       </c>
       <c r="P27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>m57</v>
       </c>
       <c r="Q27" s="1" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>m70</v>
       </c>
     </row>
@@ -1955,7 +1950,7 @@
         <v>25</v>
       </c>
       <c r="B28" t="str">
-        <f t="shared" ref="B28:B34" si="7">B18</f>
+        <f t="shared" ref="B28:B34" si="6">B18</f>
         <v>Remaining Signals</v>
       </c>
       <c r="C28" s="1">
@@ -1966,61 +1961,61 @@
         <v>0</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" ref="E28:Q28" si="8">E24</f>
+        <f t="shared" ref="E28:Q28" si="7">E24</f>
         <v>0</v>
       </c>
       <c r="F28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.166435</v>
       </c>
       <c r="G28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.13122700000000001</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>3.8631890000000002</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>0.25121500000000002</v>
       </c>
       <c r="J28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>6.1466E-2</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>3.5978000000000003E-2</v>
       </c>
       <c r="L28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>4.8861000000000002E-2</v>
       </c>
       <c r="M28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.173705</v>
       </c>
       <c r="N28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>3.4122E-2</v>
       </c>
       <c r="O28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>1.4425E-2</v>
       </c>
       <c r="P28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>-2.0010000000000002E-3</v>
       </c>
       <c r="Q28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>9.9500000000000001E-4</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B29" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>Correction factors</v>
       </c>
       <c r="C29" s="1"/>
@@ -2044,7 +2039,7 @@
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B30" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>Concentrations</v>
       </c>
       <c r="C30" s="1"/>
@@ -2068,7 +2063,7 @@
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>calculated main signal</v>
       </c>
       <c r="C31" s="1"/>
@@ -2092,7 +2087,7 @@
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>Standardized pattern</v>
       </c>
       <c r="C32" s="1"/>
@@ -2131,33 +2126,33 @@
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>Signal to subtract</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1">
-        <f t="shared" ref="E33:J33" si="9">(E32*$N$33)/$N$32</f>
+        <f t="shared" ref="E33:J33" si="8">(E32*$N$33)/$N$32</f>
         <v>5.2703338652665562E-4</v>
       </c>
       <c r="F33" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>8.2787473766769235E-3</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>1.8545383428398926E-2</v>
       </c>
       <c r="H33" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>2.8117989632322465E-3</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>2.3965853365893075E-2</v>
       </c>
       <c r="J33" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>7.7971382407698187E-2</v>
       </c>
       <c r="K33" s="1"/>
@@ -2179,32 +2174,32 @@
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="6"/>
         <v>After subtraction</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1">
-        <f t="shared" ref="D34:Q34" si="10">D28-D33</f>
+        <f t="shared" ref="D34:Q34" si="9">D28-D33</f>
         <v>0</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>-5.2703338652665562E-4</v>
       </c>
       <c r="F34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0.15815625262332308</v>
       </c>
       <c r="G34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0.11268161657160108</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>3.8603772010367678</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0.22724914663410695</v>
       </c>
       <c r="J34" s="1">
@@ -2212,93 +2207,93 @@
         <v>-1.6505382407698187E-2</v>
       </c>
       <c r="K34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>3.5978000000000003E-2</v>
       </c>
       <c r="L34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>4.791816023902478E-2</v>
       </c>
       <c r="M34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>1.1732303834351314</v>
       </c>
       <c r="N34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="O34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>1.4425E-2</v>
       </c>
       <c r="P34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>-2.0010000000000002E-3</v>
       </c>
       <c r="Q34" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>9.9500000000000001E-4</v>
       </c>
     </row>
     <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C37" s="1" t="str">
-        <f t="shared" ref="C37:Q37" si="11">C27</f>
+        <f t="shared" ref="C37:Q37" si="10">C27</f>
         <v>Time</v>
       </c>
       <c r="D37" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>m2</v>
       </c>
       <c r="E37" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>m18</v>
       </c>
       <c r="F37" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>m26</v>
       </c>
       <c r="G37" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>m27</v>
       </c>
       <c r="H37" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>m28</v>
       </c>
       <c r="I37" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>m29</v>
       </c>
       <c r="J37" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>m31</v>
       </c>
       <c r="K37" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>m39</v>
       </c>
       <c r="L37" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>m41</v>
       </c>
       <c r="M37" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>m44</v>
       </c>
       <c r="N37" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>m45</v>
       </c>
       <c r="O37" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>m56</v>
       </c>
       <c r="P37" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>m57</v>
       </c>
       <c r="Q37" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="10"/>
         <v>m70</v>
       </c>
     </row>
@@ -2307,7 +2302,7 @@
         <v>26</v>
       </c>
       <c r="B38" t="str">
-        <f t="shared" ref="B38:B44" si="12">B28</f>
+        <f t="shared" ref="B38:B44" si="11">B28</f>
         <v>Remaining Signals</v>
       </c>
       <c r="C38" s="1">
@@ -2318,61 +2313,61 @@
         <v>0</v>
       </c>
       <c r="E38" s="1">
-        <f t="shared" ref="E38:Q38" si="13">E34</f>
+        <f t="shared" ref="E38:Q38" si="12">E34</f>
         <v>-5.2703338652665562E-4</v>
       </c>
       <c r="F38" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0.15815625262332308</v>
       </c>
       <c r="G38" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0.11268161657160108</v>
       </c>
       <c r="H38" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3.8603772010367678</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0.22724914663410695</v>
       </c>
       <c r="J38" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>-1.6505382407698187E-2</v>
       </c>
       <c r="K38" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>3.5978000000000003E-2</v>
       </c>
       <c r="L38" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>4.791816023902478E-2</v>
       </c>
       <c r="M38" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.1732303834351314</v>
       </c>
       <c r="N38" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="O38" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1.4425E-2</v>
       </c>
       <c r="P38" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>-2.0010000000000002E-3</v>
       </c>
       <c r="Q38" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>9.9500000000000001E-4</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Correction factors</v>
       </c>
       <c r="C39" s="1"/>
@@ -2396,7 +2391,7 @@
     </row>
     <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Concentrations</v>
       </c>
       <c r="C40" s="1"/>
@@ -2420,7 +2415,7 @@
     </row>
     <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>calculated main signal</v>
       </c>
       <c r="C41" s="1"/>
@@ -2444,7 +2439,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Standardized pattern</v>
       </c>
       <c r="C42" s="1"/>
@@ -2491,7 +2486,7 @@
     </row>
     <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>Signal to subtract</v>
       </c>
       <c r="C43" s="1"/>
@@ -2521,156 +2516,156 @@
         <v>-1.6505382407698187E-2</v>
       </c>
       <c r="K43" s="1">
-        <f t="shared" ref="K43:Q43" si="14">(K42*$J$43)/$J$42</f>
+        <f t="shared" ref="K43:Q43" si="13">(K42*$J$43)/$J$42</f>
         <v>-2.6878195736420352E-2</v>
       </c>
       <c r="L43" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>-1.5672252008034109E-2</v>
       </c>
       <c r="M43" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>-5.2614083957049874E-3</v>
       </c>
       <c r="N43" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>-1.4902564595486059E-3</v>
       </c>
       <c r="O43" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>-2.1001397081389368E-4</v>
       </c>
       <c r="P43" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>-4.5576514771997471E-2</v>
       </c>
       <c r="Q43" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>-1.4753643925963246E-3</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>After subtraction</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1">
-        <f t="shared" ref="D44:Q44" si="15">D38-D43</f>
+        <f t="shared" ref="D44:Q44" si="14">D38-D43</f>
         <v>0</v>
       </c>
       <c r="E44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>-6.5271500216017471E-5</v>
       </c>
       <c r="F44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0.16482672597979639</v>
       </c>
       <c r="G44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0.13739407649617091</v>
       </c>
       <c r="H44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>3.8687914099489022</v>
       </c>
       <c r="I44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0.26982499555121225</v>
       </c>
       <c r="J44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="K44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>6.2856195736420359E-2</v>
       </c>
       <c r="L44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>6.3590412247058886E-2</v>
       </c>
       <c r="M44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.1784917918308364</v>
       </c>
       <c r="N44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.4902564595486059E-3</v>
       </c>
       <c r="O44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>1.4635013970813893E-2</v>
       </c>
       <c r="P44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>4.3575514771997469E-2</v>
       </c>
       <c r="Q44" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>2.4703643925963244E-3</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C46" s="1" t="str">
-        <f t="shared" ref="C46:Q46" si="16">C37</f>
+        <f t="shared" ref="C46:Q46" si="15">C37</f>
         <v>Time</v>
       </c>
       <c r="D46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>m2</v>
       </c>
       <c r="E46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>m18</v>
       </c>
       <c r="F46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>m26</v>
       </c>
       <c r="G46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>m27</v>
       </c>
       <c r="H46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>m28</v>
       </c>
       <c r="I46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>m29</v>
       </c>
       <c r="J46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>m31</v>
       </c>
       <c r="K46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>m39</v>
       </c>
       <c r="L46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>m41</v>
       </c>
       <c r="M46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>m44</v>
       </c>
       <c r="N46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>m45</v>
       </c>
       <c r="O46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>m56</v>
       </c>
       <c r="P46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>m57</v>
       </c>
       <c r="Q46" s="1" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>m70</v>
       </c>
     </row>
@@ -2691,15 +2686,15 @@
         <v>0</v>
       </c>
       <c r="E47" s="1">
-        <f t="shared" ref="E47:Q47" si="17">E44</f>
+        <f t="shared" ref="E47:Q47" si="16">E44</f>
         <v>-6.5271500216017471E-5</v>
       </c>
       <c r="F47" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0.16482672597979639</v>
       </c>
       <c r="G47" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0.13739407649617091</v>
       </c>
       <c r="H47" s="1">
@@ -2707,45 +2702,45 @@
         <v>3.8687914099489022</v>
       </c>
       <c r="I47" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0.26982499555121225</v>
       </c>
       <c r="J47" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K47" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>6.2856195736420359E-2</v>
       </c>
       <c r="L47" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>6.3590412247058886E-2</v>
       </c>
       <c r="M47" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>1.1784917918308364</v>
       </c>
       <c r="N47" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>1.4902564595486059E-3</v>
       </c>
       <c r="O47" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>1.4635013970813893E-2</v>
       </c>
       <c r="P47" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>4.3575514771997469E-2</v>
       </c>
       <c r="Q47" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>2.4703643925963244E-3</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
-        <f t="shared" ref="B48:B53" si="18">B39</f>
+        <f t="shared" ref="B48:B53" si="17">B39</f>
         <v>Correction factors</v>
       </c>
       <c r="C48" s="1"/>
@@ -2769,7 +2764,7 @@
     </row>
     <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>Concentrations</v>
       </c>
       <c r="C49" s="1"/>
@@ -2793,7 +2788,7 @@
     </row>
     <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>calculated main signal</v>
       </c>
       <c r="C50" s="1"/>
@@ -2817,7 +2812,7 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>Standardized pattern</v>
       </c>
       <c r="C51" s="1"/>
@@ -2862,33 +2857,33 @@
     </row>
     <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>Signal to subtract</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1">
-        <f t="shared" ref="E52:J52" si="19">(E51*$K$52)/$K$51</f>
+        <f t="shared" ref="E52:J52" si="18">(E51*$K$52)/$K$51</f>
         <v>3.5319240153860588E-3</v>
       </c>
       <c r="F52" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>1.5082671546125637E-2</v>
       </c>
       <c r="G52" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.1416954640458743</v>
       </c>
       <c r="H52" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>3.6067449278859902E-2</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>0.13119732421307634</v>
       </c>
       <c r="J52" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>6.9355044898693242E-3</v>
       </c>
       <c r="K52" s="1">
@@ -2919,64 +2914,64 @@
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B53" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>After subtraction</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1">
-        <f t="shared" ref="D53" si="20">D47-D52</f>
+        <f t="shared" ref="D53" si="19">D47-D52</f>
         <v>0</v>
       </c>
       <c r="E53" s="1">
-        <f t="shared" ref="E53" si="21">E47-E52</f>
+        <f t="shared" ref="E53" si="20">E47-E52</f>
         <v>-3.5971955156020763E-3</v>
       </c>
       <c r="F53" s="1">
-        <f t="shared" ref="F53" si="22">F47-F52</f>
+        <f t="shared" ref="F53" si="21">F47-F52</f>
         <v>0.14974405443367075</v>
       </c>
       <c r="G53" s="1">
-        <f t="shared" ref="G53" si="23">G47-G52</f>
+        <f t="shared" ref="G53" si="22">G47-G52</f>
         <v>-4.3013875497033838E-3</v>
       </c>
       <c r="H53" s="1">
-        <f t="shared" ref="H53" si="24">H47-H52</f>
+        <f t="shared" ref="H53" si="23">H47-H52</f>
         <v>3.8327239606700423</v>
       </c>
       <c r="I53" s="1">
-        <f t="shared" ref="I53" si="25">I47-I52</f>
+        <f t="shared" ref="I53" si="24">I47-I52</f>
         <v>0.13862767133813592</v>
       </c>
       <c r="J53" s="1">
-        <f t="shared" ref="J53" si="26">J47-J52</f>
+        <f t="shared" ref="J53" si="25">J47-J52</f>
         <v>-6.9355044898693242E-3</v>
       </c>
       <c r="K53" s="1">
-        <f t="shared" ref="K53" si="27">K47-K52</f>
+        <f t="shared" ref="K53" si="26">K47-K52</f>
         <v>0</v>
       </c>
       <c r="L53" s="1">
-        <f t="shared" ref="L53" si="28">L47-L52</f>
+        <f t="shared" ref="L53" si="27">L47-L52</f>
         <v>-0.10588535981510241</v>
       </c>
       <c r="M53" s="1">
-        <f t="shared" ref="M53" si="29">M47-M52</f>
+        <f t="shared" ref="M53" si="28">M47-M52</f>
         <v>0.88510432625577751</v>
       </c>
       <c r="N53" s="1">
-        <f t="shared" ref="N53" si="30">N47-N52</f>
+        <f t="shared" ref="N53" si="29">N47-N52</f>
         <v>-8.9509683671934147E-3</v>
       </c>
       <c r="O53" s="1">
-        <f t="shared" ref="O53" si="31">O47-O52</f>
+        <f t="shared" ref="O53" si="30">O47-O52</f>
         <v>1.3173651154412132E-2</v>
       </c>
       <c r="P53" s="1">
-        <f t="shared" ref="P53" si="32">P47-P52</f>
+        <f t="shared" ref="P53" si="31">P47-P52</f>
         <v>-5.2635551679694935E-2</v>
       </c>
       <c r="Q53" s="1">
-        <f t="shared" ref="Q53" si="33">Q47-Q52</f>
+        <f t="shared" ref="Q53" si="32">Q47-Q52</f>
         <v>2.4703643925963244E-3</v>
       </c>
     </row>
@@ -3032,7 +3027,7 @@
     </row>
     <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B57" t="str">
-        <f t="shared" ref="B57:B63" si="34">B47</f>
+        <f t="shared" ref="B57:B63" si="33">B47</f>
         <v>Remaining Signals</v>
       </c>
       <c r="C57" s="1">
@@ -3043,61 +3038,61 @@
         <v>0</v>
       </c>
       <c r="E57" s="1">
-        <f t="shared" ref="E57:Q57" si="35">E53</f>
+        <f t="shared" ref="E57:Q57" si="34">E53</f>
         <v>-3.5971955156020763E-3</v>
       </c>
       <c r="F57" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.14974405443367075</v>
       </c>
       <c r="G57" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>-4.3013875497033838E-3</v>
       </c>
       <c r="H57" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>3.8327239606700423</v>
       </c>
       <c r="I57" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.13862767133813592</v>
       </c>
       <c r="J57" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>-6.9355044898693242E-3</v>
       </c>
       <c r="K57" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="L57" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>-0.10588535981510241</v>
       </c>
       <c r="M57" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>0.88510432625577751</v>
       </c>
       <c r="N57" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>-8.9509683671934147E-3</v>
       </c>
       <c r="O57" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>1.3173651154412132E-2</v>
       </c>
       <c r="P57" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>-5.2635551679694935E-2</v>
       </c>
       <c r="Q57" s="1">
-        <f t="shared" si="35"/>
+        <f t="shared" si="34"/>
         <v>2.4703643925963244E-3</v>
       </c>
     </row>
     <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B58" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>Correction factors</v>
       </c>
       <c r="C58" s="1"/>
@@ -3121,7 +3116,7 @@
     </row>
     <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B59" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>Concentrations</v>
       </c>
       <c r="C59" s="1"/>
@@ -3145,7 +3140,7 @@
     </row>
     <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B60" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>calculated main signal</v>
       </c>
       <c r="C60" s="1"/>
@@ -3169,7 +3164,7 @@
     </row>
     <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B61" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>Standardized pattern</v>
       </c>
       <c r="C61" s="1"/>
@@ -3202,7 +3197,7 @@
     </row>
     <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B62" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>Signal to subtract</v>
       </c>
       <c r="C62" s="1"/>
@@ -3241,64 +3236,64 @@
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B63" t="str">
-        <f t="shared" si="34"/>
+        <f t="shared" si="33"/>
         <v>After subtraction</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1">
-        <f t="shared" ref="D63:Q63" si="36">D57-D62</f>
+        <f t="shared" ref="D63:Q63" si="35">D57-D62</f>
         <v>0</v>
       </c>
       <c r="E63" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>-3.5971955156020763E-3</v>
       </c>
       <c r="F63" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0.13490941013191646</v>
       </c>
       <c r="G63" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>-1.5032242396194568E-2</v>
       </c>
       <c r="H63" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>3.7481110315599673</v>
       </c>
       <c r="I63" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="J63" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>-6.9355044898693242E-3</v>
       </c>
       <c r="K63" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0</v>
       </c>
       <c r="L63" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>-0.11345518765349535</v>
       </c>
       <c r="M63" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>0.74649051907105213</v>
       </c>
       <c r="N63" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>-8.9509683671934147E-3</v>
       </c>
       <c r="O63" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>1.3173651154412132E-2</v>
       </c>
       <c r="P63" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>-5.2635551679694935E-2</v>
       </c>
       <c r="Q63" s="1">
-        <f t="shared" si="36"/>
+        <f t="shared" si="35"/>
         <v>2.4703643925963244E-3</v>
       </c>
     </row>
@@ -3366,61 +3361,61 @@
         <v>0</v>
       </c>
       <c r="E67" s="1">
-        <f t="shared" ref="E67:Q67" si="37">E63</f>
+        <f t="shared" ref="E67:Q67" si="36">E63</f>
         <v>-3.5971955156020763E-3</v>
       </c>
       <c r="F67" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0.13490941013191646</v>
       </c>
       <c r="G67" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>-1.5032242396194568E-2</v>
       </c>
       <c r="H67" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>3.7481110315599673</v>
       </c>
       <c r="I67" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="J67" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>-6.9355044898693242E-3</v>
       </c>
       <c r="K67" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="L67" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>-0.11345518765349535</v>
       </c>
       <c r="M67" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>0.74649051907105213</v>
       </c>
       <c r="N67" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>-8.9509683671934147E-3</v>
       </c>
       <c r="O67" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>1.3173651154412132E-2</v>
       </c>
       <c r="P67" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>-5.2635551679694935E-2</v>
       </c>
       <c r="Q67" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="36"/>
         <v>2.4703643925963244E-3</v>
       </c>
     </row>
     <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B68" t="str">
-        <f t="shared" ref="B68:B73" si="38">B58</f>
+        <f t="shared" ref="B68:B73" si="37">B58</f>
         <v>Correction factors</v>
       </c>
       <c r="C68" s="1"/>
@@ -3444,7 +3439,7 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B69" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>Concentrations</v>
       </c>
       <c r="C69" s="1"/>
@@ -3468,7 +3463,7 @@
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B70" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>calculated main signal</v>
       </c>
       <c r="C70" s="1"/>
@@ -3492,7 +3487,7 @@
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B71" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>Standardized pattern</v>
       </c>
       <c r="C71" s="1"/>
@@ -3521,7 +3516,7 @@
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B72" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>Signal to subtract</v>
       </c>
       <c r="C72" s="1"/>
@@ -3554,64 +3549,64 @@
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B73" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="37"/>
         <v>After subtraction</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1">
-        <f t="shared" ref="D73:Q73" si="39">D67-D72</f>
+        <f t="shared" ref="D73:Q73" si="38">D67-D72</f>
         <v>0</v>
       </c>
       <c r="E73" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>-3.5971955156020763E-3</v>
       </c>
       <c r="F73" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>0.13490941013191646</v>
       </c>
       <c r="G73" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>-1.5032242396194568E-2</v>
       </c>
       <c r="H73" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>3.6588180419960663</v>
       </c>
       <c r="I73" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>-8.9666816040954761E-4</v>
       </c>
       <c r="J73" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>-6.9355044898693242E-3</v>
       </c>
       <c r="K73" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="L73" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>-0.11345518765349535</v>
       </c>
       <c r="M73" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="N73" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>-1.783225768163809E-2</v>
       </c>
       <c r="O73" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>1.3173651154412132E-2</v>
       </c>
       <c r="P73" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>-5.2635551679694935E-2</v>
       </c>
       <c r="Q73" s="1">
-        <f t="shared" si="39"/>
+        <f t="shared" si="38"/>
         <v>2.4703643925963244E-3</v>
       </c>
     </row>
@@ -3679,61 +3674,61 @@
         <v>0</v>
       </c>
       <c r="E77" s="1">
-        <f t="shared" ref="E77:Q77" si="40">E73</f>
+        <f t="shared" ref="E77:Q77" si="39">E73</f>
         <v>-3.5971955156020763E-3</v>
       </c>
       <c r="F77" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>0.13490941013191646</v>
       </c>
       <c r="G77" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>-1.5032242396194568E-2</v>
       </c>
       <c r="H77" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>3.6588180419960663</v>
       </c>
       <c r="I77" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>-8.9666816040954761E-4</v>
       </c>
       <c r="J77" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>-6.9355044898693242E-3</v>
       </c>
       <c r="K77" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="L77" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>-0.11345518765349535</v>
       </c>
       <c r="M77" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="N77" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>-1.783225768163809E-2</v>
       </c>
       <c r="O77" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>1.3173651154412132E-2</v>
       </c>
       <c r="P77" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>-5.2635551679694935E-2</v>
       </c>
       <c r="Q77" s="1">
-        <f t="shared" si="40"/>
+        <f t="shared" si="39"/>
         <v>2.4703643925963244E-3</v>
       </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B78" t="str">
-        <f t="shared" ref="B78:B83" si="41">B68</f>
+        <f t="shared" ref="B78:B83" si="40">B68</f>
         <v>Correction factors</v>
       </c>
       <c r="C78" s="1"/>
@@ -3757,7 +3752,7 @@
     </row>
     <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B79" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>Concentrations</v>
       </c>
       <c r="C79" s="1"/>
@@ -3781,7 +3776,7 @@
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B80" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>calculated main signal</v>
       </c>
       <c r="C80" s="1"/>
@@ -3805,7 +3800,7 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B81" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>Standardized pattern</v>
       </c>
       <c r="C81" s="1"/>
@@ -3836,7 +3831,7 @@
     </row>
     <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B82" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>Signal to subtract</v>
       </c>
       <c r="C82" s="1"/>
@@ -3872,64 +3867,64 @@
     </row>
     <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B83" t="str">
-        <f t="shared" si="41"/>
+        <f t="shared" si="40"/>
         <v>After subtraction</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1">
-        <f t="shared" ref="D83:Q83" si="42">D77-D82</f>
+        <f t="shared" ref="D83:Q83" si="41">D77-D82</f>
         <v>-3.8500191582212473E-4</v>
       </c>
       <c r="E83" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>-3.5971955156020763E-3</v>
       </c>
       <c r="F83" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="G83" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>-0.17147229238325171</v>
       </c>
       <c r="H83" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>3.4117767108317549</v>
       </c>
       <c r="I83" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>-6.4945570920876116E-3</v>
       </c>
       <c r="J83" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>-6.9355044898693242E-3</v>
       </c>
       <c r="K83" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="L83" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>-0.11345518765349535</v>
       </c>
       <c r="M83" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="N83" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>-1.783225768163809E-2</v>
       </c>
       <c r="O83" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>1.3173651154412132E-2</v>
       </c>
       <c r="P83" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>-5.2635551679694935E-2</v>
       </c>
       <c r="Q83" s="1">
-        <f t="shared" si="42"/>
+        <f t="shared" si="41"/>
         <v>2.4703643925963244E-3</v>
       </c>
     </row>
@@ -3997,61 +3992,61 @@
         <v>-3.8500191582212473E-4</v>
       </c>
       <c r="E87" s="1">
-        <f t="shared" ref="E87:Q87" si="43">E83</f>
+        <f t="shared" ref="E87:Q87" si="42">E83</f>
         <v>-3.5971955156020763E-3</v>
       </c>
       <c r="F87" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="G87" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-0.17147229238325171</v>
       </c>
       <c r="H87" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>3.4117767108317549</v>
       </c>
       <c r="I87" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-6.4945570920876116E-3</v>
       </c>
       <c r="J87" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-6.9355044898693242E-3</v>
       </c>
       <c r="K87" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="L87" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-0.11345518765349535</v>
       </c>
       <c r="M87" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="N87" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-1.783225768163809E-2</v>
       </c>
       <c r="O87" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>1.3173651154412132E-2</v>
       </c>
       <c r="P87" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>-5.2635551679694935E-2</v>
       </c>
       <c r="Q87" s="1">
-        <f t="shared" si="43"/>
+        <f t="shared" si="42"/>
         <v>2.4703643925963244E-3</v>
       </c>
     </row>
     <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B88" t="str">
-        <f t="shared" ref="B88:B89" si="44">B78</f>
+        <f t="shared" ref="B88:B93" si="43">B78</f>
         <v>Correction factors</v>
       </c>
       <c r="C88" s="1"/>
@@ -4075,7 +4070,7 @@
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B89" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="43"/>
         <v>Concentrations</v>
       </c>
       <c r="C89" s="1"/>
@@ -4097,6 +4092,1761 @@
       <c r="P89" s="1"/>
       <c r="Q89" s="1"/>
     </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B90" t="str">
+        <f t="shared" si="43"/>
+        <v>calculated main signal</v>
+      </c>
+      <c r="C90" s="1"/>
+      <c r="D90" s="1"/>
+      <c r="E90" s="1"/>
+      <c r="F90" s="1"/>
+      <c r="G90" s="1"/>
+      <c r="H90" s="1">
+        <f>H89/H88</f>
+        <v>3.4117767108317549</v>
+      </c>
+      <c r="I90" s="1"/>
+      <c r="J90" s="1"/>
+      <c r="K90" s="1"/>
+      <c r="L90" s="1"/>
+      <c r="M90" s="1"/>
+      <c r="N90" s="1"/>
+      <c r="O90" s="1"/>
+      <c r="P90" s="1"/>
+      <c r="Q90" s="1"/>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B91" t="str">
+        <f t="shared" si="43"/>
+        <v>Standardized pattern</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+      <c r="H91" s="14">
+        <v>100</v>
+      </c>
+      <c r="I91" s="14">
+        <v>1.182246586</v>
+      </c>
+      <c r="J91" s="1"/>
+      <c r="K91" s="1"/>
+      <c r="L91" s="1"/>
+      <c r="M91" s="1"/>
+      <c r="N91" s="1"/>
+      <c r="O91" s="1"/>
+      <c r="P91" s="1"/>
+      <c r="Q91" s="1"/>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B92" t="str">
+        <f t="shared" si="43"/>
+        <v>Signal to subtract</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1"/>
+      <c r="E92" s="1"/>
+      <c r="F92" s="1"/>
+      <c r="G92" s="1"/>
+      <c r="H92" s="1">
+        <f>H89/H88</f>
+        <v>3.4117767108317549</v>
+      </c>
+      <c r="I92" s="1">
+        <f>(I91*$H$92)/$H$91</f>
+        <v>4.0335613685751517E-2</v>
+      </c>
+      <c r="J92" s="1"/>
+      <c r="K92" s="1"/>
+      <c r="L92" s="1"/>
+      <c r="M92" s="1"/>
+      <c r="N92" s="1"/>
+      <c r="O92" s="1"/>
+      <c r="P92" s="1"/>
+      <c r="Q92" s="1"/>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B93" t="str">
+        <f t="shared" si="43"/>
+        <v>After subtraction</v>
+      </c>
+      <c r="C93" s="1"/>
+      <c r="D93" s="1">
+        <f>D87-D92</f>
+        <v>-3.8500191582212473E-4</v>
+      </c>
+      <c r="E93" s="1">
+        <f t="shared" ref="E93:Q93" si="44">E87-E92</f>
+        <v>-3.5971955156020763E-3</v>
+      </c>
+      <c r="F93" s="1">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="G93" s="1">
+        <f t="shared" si="44"/>
+        <v>-0.17147229238325171</v>
+      </c>
+      <c r="H93" s="1">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="I93" s="1">
+        <f t="shared" si="44"/>
+        <v>-4.6830170777839131E-2</v>
+      </c>
+      <c r="J93" s="1">
+        <f t="shared" si="44"/>
+        <v>-6.9355044898693242E-3</v>
+      </c>
+      <c r="K93" s="1">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="L93" s="1">
+        <f t="shared" si="44"/>
+        <v>-0.11345518765349535</v>
+      </c>
+      <c r="M93" s="1">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+      <c r="N93" s="1">
+        <f t="shared" si="44"/>
+        <v>-1.783225768163809E-2</v>
+      </c>
+      <c r="O93" s="1">
+        <f t="shared" si="44"/>
+        <v>1.3173651154412132E-2</v>
+      </c>
+      <c r="P93" s="1">
+        <f t="shared" si="44"/>
+        <v>-5.2635551679694935E-2</v>
+      </c>
+      <c r="Q93" s="1">
+        <f t="shared" si="44"/>
+        <v>2.4703643925963244E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A96" s="19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S98" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="T98" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="U98" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>0</v>
+      </c>
+      <c r="S99" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="T99" s="6">
+        <v>31</v>
+      </c>
+      <c r="U99" s="7">
+        <v>12.380758175200878</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C100" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D100" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E100" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F100" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G100" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H100" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I100" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J100" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K100" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="L100" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M100" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N100" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O100" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P100" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q100" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="S100" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T100" s="6">
+        <v>39</v>
+      </c>
+      <c r="U100" s="8">
+        <v>12.087936672079417</v>
+      </c>
+    </row>
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>16</v>
+      </c>
+      <c r="B101" t="s">
+        <v>17</v>
+      </c>
+      <c r="C101" s="16"/>
+      <c r="D101" s="16">
+        <v>-3.8500191582212473E-4</v>
+      </c>
+      <c r="E101" s="16">
+        <v>-3.5971955156020763E-3</v>
+      </c>
+      <c r="F101" s="16">
+        <v>0</v>
+      </c>
+      <c r="G101" s="16">
+        <v>-0.17147229238325171</v>
+      </c>
+      <c r="H101" s="16">
+        <v>0</v>
+      </c>
+      <c r="I101" s="16">
+        <v>-4.6830170777839131E-2</v>
+      </c>
+      <c r="J101" s="16">
+        <v>-6.9355044898693242E-3</v>
+      </c>
+      <c r="K101" s="16">
+        <v>0</v>
+      </c>
+      <c r="L101" s="16">
+        <v>-0.11345518765349535</v>
+      </c>
+      <c r="M101" s="16">
+        <v>0</v>
+      </c>
+      <c r="N101" s="16">
+        <v>-1.783225768163809E-2</v>
+      </c>
+      <c r="O101" s="16">
+        <v>1.3173651154412132E-2</v>
+      </c>
+      <c r="P101" s="16">
+        <v>-5.2635551679694935E-2</v>
+      </c>
+      <c r="Q101" s="16">
+        <v>2.4703643925963244E-3</v>
+      </c>
+      <c r="S101" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="T101" s="6">
+        <v>45</v>
+      </c>
+      <c r="U101" s="8">
+        <v>4.8891055066059943</v>
+      </c>
+    </row>
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>18</v>
+      </c>
+      <c r="C102" s="16"/>
+      <c r="D102" s="2">
+        <v>0.55024373334910903</v>
+      </c>
+      <c r="E102" s="16"/>
+      <c r="F102" s="16"/>
+      <c r="G102" s="16"/>
+      <c r="H102" s="16"/>
+      <c r="I102" s="16"/>
+      <c r="J102" s="16"/>
+      <c r="K102" s="16"/>
+      <c r="L102" s="16"/>
+      <c r="M102" s="16"/>
+      <c r="N102" s="16"/>
+      <c r="O102" s="16"/>
+      <c r="P102" s="16"/>
+      <c r="Q102" s="16"/>
+      <c r="S102" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="T102" s="6">
+        <v>18</v>
+      </c>
+      <c r="U102" s="8">
+        <v>1.187026897776684</v>
+      </c>
+    </row>
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>19</v>
+      </c>
+      <c r="C103" s="16"/>
+      <c r="D103" s="1">
+        <f>D101*D102</f>
+        <v>-2.1184489150852533E-4</v>
+      </c>
+      <c r="E103" s="16"/>
+      <c r="F103" s="16"/>
+      <c r="G103" s="16"/>
+      <c r="H103" s="16"/>
+      <c r="I103" s="16"/>
+      <c r="J103" s="16"/>
+      <c r="K103" s="16"/>
+      <c r="L103" s="16"/>
+      <c r="M103" s="16"/>
+      <c r="N103" s="16"/>
+      <c r="O103" s="16"/>
+      <c r="P103" s="16"/>
+      <c r="Q103" s="16"/>
+      <c r="S103" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="T103" s="6">
+        <v>44</v>
+      </c>
+      <c r="U103" s="8">
+        <v>1.4227214338619145</v>
+      </c>
+    </row>
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>39</v>
+      </c>
+      <c r="D104" s="17">
+        <f>D10+D103</f>
+        <v>0.88199885969479752</v>
+      </c>
+      <c r="S104" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="T104" s="6">
+        <v>29</v>
+      </c>
+      <c r="U104" s="8">
+        <v>2.3997499909604523</v>
+      </c>
+    </row>
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S105" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="T105" s="6">
+        <v>26</v>
+      </c>
+      <c r="U105" s="8">
+        <v>3.8894768008651894</v>
+      </c>
+    </row>
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C106" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D106" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E106" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F106" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G106" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H106" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I106" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J106" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K106" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="L106" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M106" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N106" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O106" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P106" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q106" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="S106" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="T106" s="6">
+        <v>28</v>
+      </c>
+      <c r="U106" s="8">
+        <v>1.0678133917468022</v>
+      </c>
+    </row>
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>24</v>
+      </c>
+      <c r="B107" t="s">
+        <v>17</v>
+      </c>
+      <c r="C107" s="16">
+        <v>176.89449999999999</v>
+      </c>
+      <c r="D107" s="16">
+        <f>D101</f>
+        <v>-3.8500191582212473E-4</v>
+      </c>
+      <c r="E107" s="16">
+        <f>E101</f>
+        <v>-3.5971955156020763E-3</v>
+      </c>
+      <c r="F107" s="16">
+        <f>F101</f>
+        <v>0</v>
+      </c>
+      <c r="G107" s="16">
+        <f>G101</f>
+        <v>-0.17147229238325171</v>
+      </c>
+      <c r="H107" s="16">
+        <f>H101</f>
+        <v>0</v>
+      </c>
+      <c r="I107" s="16">
+        <f>I101</f>
+        <v>-4.6830170777839131E-2</v>
+      </c>
+      <c r="J107" s="16">
+        <f>J101</f>
+        <v>-6.9355044898693242E-3</v>
+      </c>
+      <c r="K107" s="16">
+        <f>K101</f>
+        <v>0</v>
+      </c>
+      <c r="L107" s="16">
+        <f>L101</f>
+        <v>-0.11345518765349535</v>
+      </c>
+      <c r="M107" s="16">
+        <f>M101</f>
+        <v>0</v>
+      </c>
+      <c r="N107" s="16">
+        <f>N101</f>
+        <v>-1.783225768163809E-2</v>
+      </c>
+      <c r="O107" s="16">
+        <f>O101</f>
+        <v>1.3173651154412132E-2</v>
+      </c>
+      <c r="P107" s="16">
+        <f>P101</f>
+        <v>-5.2635551679694935E-2</v>
+      </c>
+      <c r="Q107" s="16">
+        <f>Q101</f>
+        <v>2.4703643925963244E-3</v>
+      </c>
+      <c r="S107" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="T107" s="10">
+        <v>2</v>
+      </c>
+      <c r="U107" s="11">
+        <v>0.55856235858755843</v>
+      </c>
+    </row>
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>18</v>
+      </c>
+      <c r="C108" s="16"/>
+      <c r="D108" s="16"/>
+      <c r="E108" s="3">
+        <v>1.187026897776684</v>
+      </c>
+      <c r="F108" s="16"/>
+      <c r="G108" s="16"/>
+      <c r="H108" s="16"/>
+      <c r="I108" s="16"/>
+      <c r="J108" s="16"/>
+      <c r="K108" s="16"/>
+      <c r="L108" s="16"/>
+      <c r="M108" s="16"/>
+      <c r="N108" s="16"/>
+      <c r="O108" s="16"/>
+      <c r="P108" s="16"/>
+      <c r="Q108" s="16"/>
+    </row>
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>19</v>
+      </c>
+      <c r="C109" s="16"/>
+      <c r="D109" s="16"/>
+      <c r="E109" s="1">
+        <f>E107*E108</f>
+        <v>-4.2699678335813319E-3</v>
+      </c>
+      <c r="F109" s="16"/>
+      <c r="G109" s="16"/>
+      <c r="H109" s="16"/>
+      <c r="I109" s="16"/>
+      <c r="J109" s="16"/>
+      <c r="K109" s="16"/>
+      <c r="L109" s="16"/>
+      <c r="M109" s="16"/>
+      <c r="N109" s="16"/>
+      <c r="O109" s="16"/>
+      <c r="P109" s="16"/>
+      <c r="Q109" s="16"/>
+      <c r="S109" t="s">
+        <v>36</v>
+      </c>
+      <c r="U109" s="3"/>
+    </row>
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B110" t="s">
+        <v>39</v>
+      </c>
+      <c r="E110" s="17">
+        <f>E20+E109</f>
+        <v>0.21136771247032662</v>
+      </c>
+    </row>
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S111" t="s">
+        <v>40</v>
+      </c>
+      <c r="U111" s="1"/>
+    </row>
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C112" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D112" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E112" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F112" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G112" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H112" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I112" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J112" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K112" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="L112" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M112" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N112" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O112" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P112" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q112" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>25</v>
+      </c>
+      <c r="B113" t="s">
+        <v>17</v>
+      </c>
+      <c r="C113" s="16">
+        <v>176.89449999999999</v>
+      </c>
+      <c r="D113" s="16">
+        <f>D107</f>
+        <v>-3.8500191582212473E-4</v>
+      </c>
+      <c r="E113" s="16">
+        <f>E107</f>
+        <v>-3.5971955156020763E-3</v>
+      </c>
+      <c r="F113" s="16">
+        <f>F107</f>
+        <v>0</v>
+      </c>
+      <c r="G113" s="16">
+        <f>G107</f>
+        <v>-0.17147229238325171</v>
+      </c>
+      <c r="H113" s="16">
+        <f>H107</f>
+        <v>0</v>
+      </c>
+      <c r="I113" s="16">
+        <f>I107</f>
+        <v>-4.6830170777839131E-2</v>
+      </c>
+      <c r="J113" s="16">
+        <f>J107</f>
+        <v>-6.9355044898693242E-3</v>
+      </c>
+      <c r="K113" s="16">
+        <f>K107</f>
+        <v>0</v>
+      </c>
+      <c r="L113" s="16">
+        <f>L107</f>
+        <v>-0.11345518765349535</v>
+      </c>
+      <c r="M113" s="16">
+        <f>M107</f>
+        <v>0</v>
+      </c>
+      <c r="N113" s="16">
+        <f>N107</f>
+        <v>-1.783225768163809E-2</v>
+      </c>
+      <c r="O113" s="16">
+        <f>O107</f>
+        <v>1.3173651154412132E-2</v>
+      </c>
+      <c r="P113" s="16">
+        <f>P107</f>
+        <v>-5.2635551679694935E-2</v>
+      </c>
+      <c r="Q113" s="16">
+        <f>Q107</f>
+        <v>2.4703643925963244E-3</v>
+      </c>
+      <c r="S113" t="s">
+        <v>41</v>
+      </c>
+      <c r="U113" s="18"/>
+    </row>
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>18</v>
+      </c>
+      <c r="C114" s="16"/>
+      <c r="D114" s="16"/>
+      <c r="E114" s="16"/>
+      <c r="F114" s="16"/>
+      <c r="G114" s="16"/>
+      <c r="H114" s="16"/>
+      <c r="I114" s="16"/>
+      <c r="J114" s="16"/>
+      <c r="K114" s="16"/>
+      <c r="L114" s="16"/>
+      <c r="M114" s="16"/>
+      <c r="N114" s="3">
+        <v>4.8891055066059943</v>
+      </c>
+      <c r="O114" s="16"/>
+      <c r="P114" s="16"/>
+      <c r="Q114" s="16"/>
+    </row>
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>19</v>
+      </c>
+      <c r="C115" s="16"/>
+      <c r="D115" s="16"/>
+      <c r="E115" s="16"/>
+      <c r="F115" s="16"/>
+      <c r="G115" s="16"/>
+      <c r="H115" s="16"/>
+      <c r="I115" s="16"/>
+      <c r="J115" s="16"/>
+      <c r="K115" s="16"/>
+      <c r="L115" s="16"/>
+      <c r="M115" s="16"/>
+      <c r="N115" s="1">
+        <f>N113*N114</f>
+        <v>-8.7183789226513833E-2</v>
+      </c>
+      <c r="O115" s="16"/>
+      <c r="P115" s="16"/>
+      <c r="Q115" s="16"/>
+    </row>
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>39</v>
+      </c>
+      <c r="N116" s="17">
+        <f>N30+N115</f>
+        <v>7.9642268869895907E-2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C118" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D118" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E118" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F118" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G118" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H118" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I118" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J118" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K118" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="L118" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M118" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N118" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O118" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P118" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q118" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>26</v>
+      </c>
+      <c r="B119" t="s">
+        <v>17</v>
+      </c>
+      <c r="C119" s="16">
+        <v>176.89449999999999</v>
+      </c>
+      <c r="D119" s="16">
+        <f>D113</f>
+        <v>-3.8500191582212473E-4</v>
+      </c>
+      <c r="E119" s="16">
+        <f>E113</f>
+        <v>-3.5971955156020763E-3</v>
+      </c>
+      <c r="F119" s="16">
+        <f>F113</f>
+        <v>0</v>
+      </c>
+      <c r="G119" s="16">
+        <f>G113</f>
+        <v>-0.17147229238325171</v>
+      </c>
+      <c r="H119" s="16">
+        <f>H113</f>
+        <v>0</v>
+      </c>
+      <c r="I119" s="16">
+        <f>I113</f>
+        <v>-4.6830170777839131E-2</v>
+      </c>
+      <c r="J119" s="16">
+        <f>J113</f>
+        <v>-6.9355044898693242E-3</v>
+      </c>
+      <c r="K119" s="16">
+        <f>K113</f>
+        <v>0</v>
+      </c>
+      <c r="L119" s="16">
+        <f>L113</f>
+        <v>-0.11345518765349535</v>
+      </c>
+      <c r="M119" s="16">
+        <f>M113</f>
+        <v>0</v>
+      </c>
+      <c r="N119" s="16">
+        <f>N113</f>
+        <v>-1.783225768163809E-2</v>
+      </c>
+      <c r="O119" s="16">
+        <f>O113</f>
+        <v>1.3173651154412132E-2</v>
+      </c>
+      <c r="P119" s="16">
+        <f>P113</f>
+        <v>-5.2635551679694935E-2</v>
+      </c>
+      <c r="Q119" s="16">
+        <f>Q113</f>
+        <v>2.4703643925963244E-3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>18</v>
+      </c>
+      <c r="C120" s="16"/>
+      <c r="D120" s="16"/>
+      <c r="E120" s="16"/>
+      <c r="F120" s="16"/>
+      <c r="G120" s="16"/>
+      <c r="H120" s="16"/>
+      <c r="I120" s="16"/>
+      <c r="J120" s="3">
+        <v>12.380758175200878</v>
+      </c>
+      <c r="K120" s="16"/>
+      <c r="L120" s="16"/>
+      <c r="M120" s="16"/>
+      <c r="N120" s="16"/>
+      <c r="O120" s="16"/>
+      <c r="P120" s="16"/>
+      <c r="Q120" s="16"/>
+    </row>
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>19</v>
+      </c>
+      <c r="C121" s="16"/>
+      <c r="D121" s="16"/>
+      <c r="E121" s="16"/>
+      <c r="F121" s="16"/>
+      <c r="G121" s="16"/>
+      <c r="H121" s="16"/>
+      <c r="I121" s="16"/>
+      <c r="J121" s="1">
+        <f>J119*J120</f>
+        <v>-8.5866803912092032E-2</v>
+      </c>
+      <c r="K121" s="16"/>
+      <c r="L121" s="16"/>
+      <c r="M121" s="16"/>
+      <c r="N121" s="16"/>
+      <c r="O121" s="16"/>
+      <c r="P121" s="16"/>
+      <c r="Q121" s="16"/>
+    </row>
+    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>39</v>
+      </c>
+      <c r="J122" s="17">
+        <f>J40+J121</f>
+        <v>-0.29021595209101814</v>
+      </c>
+    </row>
+    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C124" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D124" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E124" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F124" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G124" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H124" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I124" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J124" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K124" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="L124" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M124" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N124" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O124" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P124" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q124" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>27</v>
+      </c>
+      <c r="B125" t="s">
+        <v>17</v>
+      </c>
+      <c r="C125" s="16">
+        <v>176.89449999999999</v>
+      </c>
+      <c r="D125" s="16">
+        <f>D119</f>
+        <v>-3.8500191582212473E-4</v>
+      </c>
+      <c r="E125" s="16">
+        <f>E119</f>
+        <v>-3.5971955156020763E-3</v>
+      </c>
+      <c r="F125" s="16">
+        <f>F119</f>
+        <v>0</v>
+      </c>
+      <c r="G125" s="16">
+        <f>G119</f>
+        <v>-0.17147229238325171</v>
+      </c>
+      <c r="H125" s="16">
+        <f>H119</f>
+        <v>0</v>
+      </c>
+      <c r="I125" s="16">
+        <f>I119</f>
+        <v>-4.6830170777839131E-2</v>
+      </c>
+      <c r="J125" s="16">
+        <f>J119</f>
+        <v>-6.9355044898693242E-3</v>
+      </c>
+      <c r="K125" s="16">
+        <f>K119</f>
+        <v>0</v>
+      </c>
+      <c r="L125" s="16">
+        <f>L119</f>
+        <v>-0.11345518765349535</v>
+      </c>
+      <c r="M125" s="16">
+        <f>M119</f>
+        <v>0</v>
+      </c>
+      <c r="N125" s="16">
+        <f>N119</f>
+        <v>-1.783225768163809E-2</v>
+      </c>
+      <c r="O125" s="16">
+        <f>O119</f>
+        <v>1.3173651154412132E-2</v>
+      </c>
+      <c r="P125" s="16">
+        <f>P119</f>
+        <v>-5.2635551679694935E-2</v>
+      </c>
+      <c r="Q125" s="16">
+        <f>Q119</f>
+        <v>2.4703643925963244E-3</v>
+      </c>
+    </row>
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>18</v>
+      </c>
+      <c r="C126" s="16"/>
+      <c r="D126" s="16"/>
+      <c r="E126" s="16"/>
+      <c r="F126" s="16"/>
+      <c r="G126" s="16"/>
+      <c r="H126" s="16"/>
+      <c r="I126" s="16"/>
+      <c r="J126" s="16"/>
+      <c r="K126" s="3">
+        <v>12.087936672079417</v>
+      </c>
+      <c r="L126" s="16"/>
+      <c r="M126" s="16"/>
+      <c r="N126" s="16"/>
+      <c r="O126" s="16"/>
+      <c r="P126" s="16"/>
+      <c r="Q126" s="16"/>
+    </row>
+    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>19</v>
+      </c>
+      <c r="C127" s="16"/>
+      <c r="D127" s="16"/>
+      <c r="E127" s="16"/>
+      <c r="F127" s="16"/>
+      <c r="G127" s="16"/>
+      <c r="H127" s="16"/>
+      <c r="I127" s="16"/>
+      <c r="J127" s="16"/>
+      <c r="K127" s="1">
+        <f>K125*K126</f>
+        <v>0</v>
+      </c>
+      <c r="L127" s="16"/>
+      <c r="M127" s="16"/>
+      <c r="N127" s="16"/>
+      <c r="O127" s="16"/>
+      <c r="P127" s="16"/>
+      <c r="Q127" s="16"/>
+    </row>
+    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>39</v>
+      </c>
+      <c r="K128" s="17">
+        <f>K49+K127</f>
+        <v>0.75980171350967751</v>
+      </c>
+    </row>
+    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C130" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D130" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E130" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F130" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G130" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H130" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I130" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J130" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K130" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="L130" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M130" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N130" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O130" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P130" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q130" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>32</v>
+      </c>
+      <c r="B131" t="s">
+        <v>17</v>
+      </c>
+      <c r="C131" s="16">
+        <v>176.89449999999999</v>
+      </c>
+      <c r="D131" s="16">
+        <f>D125</f>
+        <v>-3.8500191582212473E-4</v>
+      </c>
+      <c r="E131" s="16">
+        <f>E125</f>
+        <v>-3.5971955156020763E-3</v>
+      </c>
+      <c r="F131" s="16">
+        <f>F125</f>
+        <v>0</v>
+      </c>
+      <c r="G131" s="16">
+        <f>G125</f>
+        <v>-0.17147229238325171</v>
+      </c>
+      <c r="H131" s="16">
+        <f>H125</f>
+        <v>0</v>
+      </c>
+      <c r="I131" s="16">
+        <f>I125</f>
+        <v>-4.6830170777839131E-2</v>
+      </c>
+      <c r="J131" s="16">
+        <f>J125</f>
+        <v>-6.9355044898693242E-3</v>
+      </c>
+      <c r="K131" s="16">
+        <f>K125</f>
+        <v>0</v>
+      </c>
+      <c r="L131" s="16">
+        <f>L125</f>
+        <v>-0.11345518765349535</v>
+      </c>
+      <c r="M131" s="16">
+        <f>M125</f>
+        <v>0</v>
+      </c>
+      <c r="N131" s="16">
+        <f>N125</f>
+        <v>-1.783225768163809E-2</v>
+      </c>
+      <c r="O131" s="16">
+        <f>O125</f>
+        <v>1.3173651154412132E-2</v>
+      </c>
+      <c r="P131" s="16">
+        <f>P125</f>
+        <v>-5.2635551679694935E-2</v>
+      </c>
+      <c r="Q131" s="16">
+        <f>Q125</f>
+        <v>2.4703643925963244E-3</v>
+      </c>
+    </row>
+    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>18</v>
+      </c>
+      <c r="C132" s="16"/>
+      <c r="D132" s="16"/>
+      <c r="E132" s="16"/>
+      <c r="F132" s="16"/>
+      <c r="G132" s="16"/>
+      <c r="H132" s="16"/>
+      <c r="I132" s="3">
+        <v>2.3997499909604523</v>
+      </c>
+      <c r="J132" s="16"/>
+      <c r="K132" s="16"/>
+      <c r="L132" s="16"/>
+      <c r="M132" s="16"/>
+      <c r="N132" s="16"/>
+      <c r="O132" s="16"/>
+      <c r="P132" s="16"/>
+      <c r="Q132" s="16"/>
+    </row>
+    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>19</v>
+      </c>
+      <c r="C133" s="16"/>
+      <c r="D133" s="16"/>
+      <c r="E133" s="16"/>
+      <c r="F133" s="16"/>
+      <c r="G133" s="16"/>
+      <c r="H133" s="16"/>
+      <c r="I133" s="1">
+        <f>I131*I132</f>
+        <v>-0.1123807019007959</v>
+      </c>
+      <c r="J133" s="16"/>
+      <c r="K133" s="16"/>
+      <c r="L133" s="16"/>
+      <c r="M133" s="16"/>
+      <c r="N133" s="16"/>
+      <c r="O133" s="16"/>
+      <c r="P133" s="16"/>
+      <c r="Q133" s="16"/>
+    </row>
+    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>39</v>
+      </c>
+      <c r="I134" s="17">
+        <f>I59+I133</f>
+        <v>0.22029105113976433</v>
+      </c>
+    </row>
+    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C136" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D136" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E136" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F136" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G136" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H136" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I136" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J136" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K136" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="L136" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M136" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N136" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O136" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P136" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q136" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>31</v>
+      </c>
+      <c r="B137" t="s">
+        <v>17</v>
+      </c>
+      <c r="C137" s="16">
+        <v>176.89449999999999</v>
+      </c>
+      <c r="D137" s="16">
+        <f>D131</f>
+        <v>-3.8500191582212473E-4</v>
+      </c>
+      <c r="E137" s="16">
+        <f>E131</f>
+        <v>-3.5971955156020763E-3</v>
+      </c>
+      <c r="F137" s="16">
+        <f>F131</f>
+        <v>0</v>
+      </c>
+      <c r="G137" s="16">
+        <f>G131</f>
+        <v>-0.17147229238325171</v>
+      </c>
+      <c r="H137" s="16">
+        <f>H131</f>
+        <v>0</v>
+      </c>
+      <c r="I137" s="16">
+        <f>I131</f>
+        <v>-4.6830170777839131E-2</v>
+      </c>
+      <c r="J137" s="16">
+        <f>J131</f>
+        <v>-6.9355044898693242E-3</v>
+      </c>
+      <c r="K137" s="16">
+        <f>K131</f>
+        <v>0</v>
+      </c>
+      <c r="L137" s="16">
+        <f>L131</f>
+        <v>-0.11345518765349535</v>
+      </c>
+      <c r="M137" s="16">
+        <f>M131</f>
+        <v>0</v>
+      </c>
+      <c r="N137" s="16">
+        <f>N131</f>
+        <v>-1.783225768163809E-2</v>
+      </c>
+      <c r="O137" s="16">
+        <f>O131</f>
+        <v>1.3173651154412132E-2</v>
+      </c>
+      <c r="P137" s="16">
+        <f>P131</f>
+        <v>-5.2635551679694935E-2</v>
+      </c>
+      <c r="Q137" s="16">
+        <f>Q131</f>
+        <v>2.4703643925963244E-3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>18</v>
+      </c>
+      <c r="C138" s="16"/>
+      <c r="D138" s="16"/>
+      <c r="E138" s="16"/>
+      <c r="F138" s="16"/>
+      <c r="G138" s="16"/>
+      <c r="H138" s="16"/>
+      <c r="I138" s="16"/>
+      <c r="J138" s="16"/>
+      <c r="K138" s="16"/>
+      <c r="L138" s="16"/>
+      <c r="M138" s="3">
+        <v>1.4227214338619145</v>
+      </c>
+      <c r="N138" s="16"/>
+      <c r="O138" s="16"/>
+      <c r="P138" s="16"/>
+      <c r="Q138" s="16"/>
+    </row>
+    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>19</v>
+      </c>
+      <c r="C139" s="16"/>
+      <c r="D139" s="16"/>
+      <c r="E139" s="16"/>
+      <c r="F139" s="16"/>
+      <c r="G139" s="16"/>
+      <c r="H139" s="16"/>
+      <c r="I139" s="16"/>
+      <c r="J139" s="16"/>
+      <c r="K139" s="16"/>
+      <c r="L139" s="16"/>
+      <c r="M139" s="1">
+        <f>M137*M138</f>
+        <v>0</v>
+      </c>
+      <c r="N139" s="16"/>
+      <c r="O139" s="16"/>
+      <c r="P139" s="16"/>
+      <c r="Q139" s="16"/>
+    </row>
+    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>39</v>
+      </c>
+      <c r="M140" s="17">
+        <f>M69+M139</f>
+        <v>1.0620480616570922</v>
+      </c>
+    </row>
+    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C142" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D142" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E142" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F142" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G142" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H142" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I142" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J142" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K142" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="L142" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M142" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N142" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O142" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P142" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q142" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>35</v>
+      </c>
+      <c r="B143" t="s">
+        <v>17</v>
+      </c>
+      <c r="C143" s="16">
+        <v>176.89449999999999</v>
+      </c>
+      <c r="D143" s="16">
+        <f>D137</f>
+        <v>-3.8500191582212473E-4</v>
+      </c>
+      <c r="E143" s="16">
+        <f>E137</f>
+        <v>-3.5971955156020763E-3</v>
+      </c>
+      <c r="F143" s="16">
+        <f>F137</f>
+        <v>0</v>
+      </c>
+      <c r="G143" s="16">
+        <f>G137</f>
+        <v>-0.17147229238325171</v>
+      </c>
+      <c r="H143" s="16">
+        <f>H137</f>
+        <v>0</v>
+      </c>
+      <c r="I143" s="16">
+        <f>I137</f>
+        <v>-4.6830170777839131E-2</v>
+      </c>
+      <c r="J143" s="16">
+        <f>J137</f>
+        <v>-6.9355044898693242E-3</v>
+      </c>
+      <c r="K143" s="16">
+        <f>K137</f>
+        <v>0</v>
+      </c>
+      <c r="L143" s="16">
+        <f>L137</f>
+        <v>-0.11345518765349535</v>
+      </c>
+      <c r="M143" s="16">
+        <f>M137</f>
+        <v>0</v>
+      </c>
+      <c r="N143" s="16">
+        <f>N137</f>
+        <v>-1.783225768163809E-2</v>
+      </c>
+      <c r="O143" s="16">
+        <f>O137</f>
+        <v>1.3173651154412132E-2</v>
+      </c>
+      <c r="P143" s="16">
+        <f>P137</f>
+        <v>-5.2635551679694935E-2</v>
+      </c>
+      <c r="Q143" s="16">
+        <f>Q137</f>
+        <v>2.4703643925963244E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>18</v>
+      </c>
+      <c r="C144" s="16"/>
+      <c r="D144" s="16"/>
+      <c r="E144" s="16"/>
+      <c r="F144" s="3">
+        <f>U105</f>
+        <v>3.8894768008651894</v>
+      </c>
+      <c r="G144" s="16"/>
+      <c r="H144" s="16"/>
+      <c r="I144" s="16"/>
+      <c r="J144" s="16"/>
+      <c r="K144" s="16"/>
+      <c r="L144" s="16"/>
+      <c r="M144" s="16"/>
+      <c r="N144" s="16"/>
+      <c r="O144" s="16"/>
+      <c r="P144" s="16"/>
+      <c r="Q144" s="16"/>
+    </row>
+    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>19</v>
+      </c>
+      <c r="C145" s="16"/>
+      <c r="D145" s="16"/>
+      <c r="E145" s="16"/>
+      <c r="F145" s="1">
+        <f>F143*F144</f>
+        <v>0</v>
+      </c>
+      <c r="G145" s="16"/>
+      <c r="H145" s="16"/>
+      <c r="I145" s="16"/>
+      <c r="J145" s="16"/>
+      <c r="K145" s="16"/>
+      <c r="L145" s="16"/>
+      <c r="M145" s="16"/>
+      <c r="N145" s="16"/>
+      <c r="O145" s="16"/>
+      <c r="P145" s="16"/>
+      <c r="Q145" s="16"/>
+    </row>
+    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>39</v>
+      </c>
+      <c r="F146" s="17">
+        <f>F79+F145</f>
+        <v>0.52472702092649615</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C148" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D148" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E148" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F148" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G148" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="H148" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I148" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="J148" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="K148" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="L148" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M148" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="N148" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="O148" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P148" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q148" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>34</v>
+      </c>
+      <c r="B149" t="s">
+        <v>17</v>
+      </c>
+      <c r="C149" s="16">
+        <v>176.89449999999999</v>
+      </c>
+      <c r="D149" s="16">
+        <f>D143</f>
+        <v>-3.8500191582212473E-4</v>
+      </c>
+      <c r="E149" s="16">
+        <f t="shared" ref="E149:Q149" si="45">E143</f>
+        <v>-3.5971955156020763E-3</v>
+      </c>
+      <c r="F149" s="16">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="G149" s="16">
+        <f t="shared" si="45"/>
+        <v>-0.17147229238325171</v>
+      </c>
+      <c r="H149" s="16">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="I149" s="16">
+        <f t="shared" si="45"/>
+        <v>-4.6830170777839131E-2</v>
+      </c>
+      <c r="J149" s="16">
+        <f t="shared" si="45"/>
+        <v>-6.9355044898693242E-3</v>
+      </c>
+      <c r="K149" s="16">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="L149" s="16">
+        <f t="shared" si="45"/>
+        <v>-0.11345518765349535</v>
+      </c>
+      <c r="M149" s="16">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="N149" s="16">
+        <f t="shared" si="45"/>
+        <v>-1.783225768163809E-2</v>
+      </c>
+      <c r="O149" s="16">
+        <f t="shared" si="45"/>
+        <v>1.3173651154412132E-2</v>
+      </c>
+      <c r="P149" s="16">
+        <f t="shared" si="45"/>
+        <v>-5.2635551679694935E-2</v>
+      </c>
+      <c r="Q149" s="16">
+        <f t="shared" si="45"/>
+        <v>2.4703643925963244E-3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>18</v>
+      </c>
+      <c r="C150" s="16"/>
+      <c r="D150" s="16"/>
+      <c r="E150" s="16"/>
+      <c r="F150" s="16"/>
+      <c r="G150" s="16"/>
+      <c r="H150" s="3">
+        <f>U106</f>
+        <v>1.0678133917468022</v>
+      </c>
+      <c r="I150" s="16"/>
+      <c r="J150" s="16"/>
+      <c r="K150" s="16"/>
+      <c r="L150" s="16"/>
+      <c r="M150" s="16"/>
+      <c r="N150" s="16"/>
+      <c r="O150" s="16"/>
+      <c r="P150" s="16"/>
+      <c r="Q150" s="16"/>
+    </row>
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>19</v>
+      </c>
+      <c r="C151" s="16"/>
+      <c r="D151" s="16"/>
+      <c r="E151" s="16"/>
+      <c r="F151" s="16"/>
+      <c r="G151" s="16"/>
+      <c r="H151" s="1">
+        <f>H149*H150</f>
+        <v>0</v>
+      </c>
+      <c r="I151" s="16"/>
+      <c r="J151" s="16"/>
+      <c r="K151" s="16"/>
+      <c r="L151" s="16"/>
+      <c r="M151" s="16"/>
+      <c r="N151" s="16"/>
+      <c r="O151" s="16"/>
+      <c r="P151" s="16"/>
+      <c r="Q151" s="16"/>
+    </row>
+    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>39</v>
+      </c>
+      <c r="H152" s="17">
+        <f>H89+H151</f>
+        <v>3.643140861476005</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Grammatical Error Fix "Test_11_SLS_Implicit.xlsx"
</commit_message>
<xml_diff>
--- a/UnitTests/TuningCorrector/test_11 Manual SLS Implicit/9/Test_11_SLS_Implicit.xlsx
+++ b/UnitTests/TuningCorrector/test_11 Manual SLS Implicit/9/Test_11_SLS_Implicit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f4bda48a8e8bf62b/2021LaneLeeCCIFall2021/Data Analysis/220310_Implicit_SLS_Unit_Test_11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="672" documentId="13_ncr:40009_{2AE2FE10-F754-4E12-AD7D-77D7A5496061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{562F133D-9E4B-465B-BD10-3ADEB08D383B}"/>
+  <xr:revisionPtr revIDLastSave="682" documentId="13_ncr:40009_{2AE2FE10-F754-4E12-AD7D-77D7A5496061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BFAD382-E3FD-4A8C-8D40-F6B62DAD0A69}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="45" windowWidth="32130" windowHeight="14520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -150,16 +150,16 @@
     <t>Unit Test 10 Manual SLS:</t>
   </si>
   <si>
-    <t>SLS Implicit Concetration</t>
-  </si>
-  <si>
     <t xml:space="preserve">Implicit SLS Concentration to be added: </t>
   </si>
   <si>
-    <t>Final Calculated Molecule Concetration:</t>
+    <t>Performing SLS Implicit:</t>
   </si>
   <si>
-    <t>Performing SLS Implicit:</t>
+    <t>SLS Implicit Concentration</t>
+  </si>
+  <si>
+    <t>Final Calculated Molecule Concentration:</t>
   </si>
 </sst>
 </file>
@@ -1167,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:V152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N96" sqref="N96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4233,7 +4233,7 @@
     </row>
     <row r="96" spans="1:17" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A96" s="19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.25">
@@ -4442,7 +4442,7 @@
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D104" s="17">
         <f>D10+D103</f>
@@ -4652,7 +4652,7 @@
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="E110" s="17">
         <f>E20+E109</f>
@@ -4661,7 +4661,7 @@
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S111" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U111" s="1"/>
     </row>
@@ -4779,7 +4779,7 @@
         <v>2.4703643925963244E-3</v>
       </c>
       <c r="S113" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="U113" s="18"/>
     </row>
@@ -4830,7 +4830,7 @@
     </row>
     <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="N116" s="17">
         <f>N30+N115</f>
@@ -4998,7 +4998,7 @@
     </row>
     <row r="122" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="J122" s="17">
         <f>J40+J121</f>
@@ -5166,7 +5166,7 @@
     </row>
     <row r="128" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K128" s="17">
         <f>K49+K127</f>
@@ -5334,7 +5334,7 @@
     </row>
     <row r="134" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I134" s="17">
         <f>I59+I133</f>
@@ -5502,7 +5502,7 @@
     </row>
     <row r="140" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M140" s="17">
         <f>M69+M139</f>
@@ -5671,7 +5671,7 @@
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F146" s="17">
         <f>F79+F145</f>
@@ -5840,7 +5840,7 @@
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H152" s="17">
         <f>H89+H151</f>

</xml_diff>